<commit_message>
Update ETND_ 케이블20241016.xlsx and convert to CSV
</commit_message>
<xml_diff>
--- a/ETND_ 케이블20241016.xlsx
+++ b/ETND_ 케이블20241016.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/JDS_BU/Git_Hub/GIC_HONGKONG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69629E3C-E6E9-FA45-BC73-F5A8589ADA22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F8BAF7-0063-0046-B7D1-62E1A9B11B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3740" yWindow="780" windowWidth="34260" windowHeight="24840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="101">
   <si>
     <t>Pin map</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -448,6 +448,10 @@
   </si>
   <si>
     <t>5 / DC 110V</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>aaaaa</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -919,7 +923,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="188">
+  <cellXfs count="189">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1268,6 +1272,210 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="7" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -1277,212 +1485,11 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="7" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3295,10 +3302,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q156"/>
+  <dimension ref="A1:W156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="29" zoomScaleNormal="90" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="D156" sqref="D156"/>
+      <selection activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="17" outlineLevelRow="1"/>
@@ -3320,38 +3327,38 @@
     <col min="17" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="22">
+    <row r="1" spans="1:23" ht="22">
       <c r="A1" s="40"/>
-      <c r="B1" s="173" t="s">
+      <c r="B1" s="128" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="173"/>
-      <c r="D1" s="173"/>
-      <c r="E1" s="173"/>
-      <c r="F1" s="173"/>
-      <c r="G1" s="173"/>
-      <c r="H1" s="173"/>
-      <c r="I1" s="173"/>
-      <c r="J1" s="173"/>
-      <c r="K1" s="173"/>
-      <c r="L1" s="173"/>
-      <c r="M1" s="173"/>
-      <c r="N1" s="173"/>
-      <c r="O1" s="173"/>
+      <c r="C1" s="128"/>
+      <c r="D1" s="128"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="128"/>
+      <c r="G1" s="128"/>
+      <c r="H1" s="128"/>
+      <c r="I1" s="128"/>
+      <c r="J1" s="128"/>
+      <c r="K1" s="128"/>
+      <c r="L1" s="128"/>
+      <c r="M1" s="128"/>
+      <c r="N1" s="128"/>
+      <c r="O1" s="128"/>
       <c r="P1" s="1"/>
     </row>
-    <row r="2" spans="1:16" outlineLevel="1">
+    <row r="2" spans="1:23" outlineLevel="1">
       <c r="A2" s="41"/>
       <c r="P2" s="5"/>
     </row>
-    <row r="3" spans="1:16" outlineLevel="1">
+    <row r="3" spans="1:23" outlineLevel="1">
       <c r="A3" s="41"/>
       <c r="B3" s="42" t="s">
         <v>0</v>
       </c>
       <c r="P3" s="5"/>
     </row>
-    <row r="4" spans="1:16" s="6" customFormat="1" ht="27" customHeight="1" outlineLevel="1">
+    <row r="4" spans="1:23" s="6" customFormat="1" ht="27" customHeight="1" outlineLevel="1">
       <c r="A4" s="43"/>
       <c r="B4" s="18" t="s">
         <v>1</v>
@@ -3359,28 +3366,28 @@
       <c r="C4" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="139" t="s">
+      <c r="D4" s="129" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="139"/>
+      <c r="E4" s="129"/>
       <c r="F4" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="139" t="s">
+      <c r="G4" s="129" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="139"/>
-      <c r="I4" s="139"/>
+      <c r="H4" s="129"/>
+      <c r="I4" s="129"/>
       <c r="J4" s="34" t="s">
         <v>6</v>
       </c>
       <c r="K4" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="139" t="s">
+      <c r="L4" s="129" t="s">
         <v>3</v>
       </c>
-      <c r="M4" s="139"/>
+      <c r="M4" s="129"/>
       <c r="N4" s="34" t="s">
         <v>2</v>
       </c>
@@ -3389,56 +3396,59 @@
       </c>
       <c r="P4" s="7"/>
     </row>
-    <row r="5" spans="1:16" ht="16.5" customHeight="1" outlineLevel="1">
+    <row r="5" spans="1:23" ht="16.5" customHeight="1" outlineLevel="1">
       <c r="A5" s="41"/>
-      <c r="B5" s="174" t="s">
+      <c r="B5" s="130" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="143" t="s">
+      <c r="C5" s="165" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="175">
+      <c r="D5" s="132">
         <v>1</v>
       </c>
-      <c r="E5" s="175"/>
+      <c r="E5" s="132"/>
       <c r="F5" s="67"/>
-      <c r="G5" s="153" t="s">
+      <c r="G5" s="131" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="153"/>
-      <c r="I5" s="153"/>
+      <c r="H5" s="131"/>
+      <c r="I5" s="131"/>
       <c r="J5" s="68" t="s">
         <v>86</v>
       </c>
       <c r="K5" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="L5" s="175">
+      <c r="L5" s="132">
         <v>4</v>
       </c>
-      <c r="M5" s="175"/>
-      <c r="N5" s="174" t="s">
+      <c r="M5" s="132"/>
+      <c r="N5" s="130" t="s">
         <v>45</v>
       </c>
-      <c r="O5" s="152" t="s">
+      <c r="O5" s="133" t="s">
         <v>93</v>
       </c>
       <c r="P5" s="5"/>
-    </row>
-    <row r="6" spans="1:16" ht="16.5" customHeight="1" outlineLevel="1">
+      <c r="W5" s="188" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="16.5" customHeight="1" outlineLevel="1">
       <c r="A6" s="41"/>
-      <c r="B6" s="174"/>
-      <c r="C6" s="144"/>
-      <c r="D6" s="175">
+      <c r="B6" s="130"/>
+      <c r="C6" s="166"/>
+      <c r="D6" s="132">
         <v>3</v>
       </c>
-      <c r="E6" s="175"/>
+      <c r="E6" s="132"/>
       <c r="F6" s="65"/>
-      <c r="G6" s="176" t="s">
+      <c r="G6" s="135" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="177"/>
-      <c r="I6" s="178"/>
+      <c r="H6" s="136"/>
+      <c r="I6" s="137"/>
       <c r="J6" s="66" t="str">
         <f>J5</f>
         <v>800+350mm</v>
@@ -3446,28 +3456,28 @@
       <c r="K6" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="L6" s="175">
+      <c r="L6" s="132">
         <v>3</v>
       </c>
-      <c r="M6" s="175"/>
-      <c r="N6" s="175"/>
-      <c r="O6" s="152"/>
+      <c r="M6" s="132"/>
+      <c r="N6" s="132"/>
+      <c r="O6" s="133"/>
       <c r="P6" s="5"/>
     </row>
-    <row r="7" spans="1:16" ht="16.5" customHeight="1" outlineLevel="1">
+    <row r="7" spans="1:23" ht="16.5" customHeight="1" outlineLevel="1">
       <c r="A7" s="41"/>
-      <c r="B7" s="174"/>
-      <c r="C7" s="144"/>
-      <c r="D7" s="175">
+      <c r="B7" s="130"/>
+      <c r="C7" s="166"/>
+      <c r="D7" s="132">
         <v>2</v>
       </c>
-      <c r="E7" s="175"/>
+      <c r="E7" s="132"/>
       <c r="F7" s="112"/>
-      <c r="G7" s="142" t="s">
+      <c r="G7" s="134" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="142"/>
-      <c r="I7" s="142"/>
+      <c r="H7" s="134"/>
+      <c r="I7" s="134"/>
       <c r="J7" s="113" t="str">
         <f>J5</f>
         <v>800+350mm</v>
@@ -3475,28 +3485,28 @@
       <c r="K7" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="L7" s="175">
+      <c r="L7" s="132">
         <v>2</v>
       </c>
-      <c r="M7" s="175"/>
-      <c r="N7" s="175"/>
-      <c r="O7" s="152"/>
+      <c r="M7" s="132"/>
+      <c r="N7" s="132"/>
+      <c r="O7" s="133"/>
       <c r="P7" s="5"/>
     </row>
-    <row r="8" spans="1:16" ht="16.5" customHeight="1" outlineLevel="1">
+    <row r="8" spans="1:23" ht="16.5" customHeight="1" outlineLevel="1">
       <c r="A8" s="41"/>
-      <c r="B8" s="174"/>
-      <c r="C8" s="145"/>
-      <c r="D8" s="175">
+      <c r="B8" s="130"/>
+      <c r="C8" s="167"/>
+      <c r="D8" s="132">
         <v>4</v>
       </c>
-      <c r="E8" s="175"/>
+      <c r="E8" s="132"/>
       <c r="F8" s="69"/>
-      <c r="G8" s="179" t="s">
+      <c r="G8" s="138" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="179"/>
-      <c r="I8" s="179"/>
+      <c r="H8" s="138"/>
+      <c r="I8" s="138"/>
       <c r="J8" s="70" t="str">
         <f>J5</f>
         <v>800+350mm</v>
@@ -3504,94 +3514,94 @@
       <c r="K8" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="L8" s="175">
+      <c r="L8" s="132">
         <v>1</v>
       </c>
-      <c r="M8" s="175"/>
-      <c r="N8" s="175"/>
-      <c r="O8" s="152"/>
+      <c r="M8" s="132"/>
+      <c r="N8" s="132"/>
+      <c r="O8" s="133"/>
       <c r="P8" s="5"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:23">
       <c r="A9" s="41"/>
       <c r="P9" s="5"/>
     </row>
-    <row r="10" spans="1:16" s="76" customFormat="1" ht="16.5" customHeight="1" outlineLevel="1">
+    <row r="10" spans="1:23" s="76" customFormat="1" ht="16.5" customHeight="1" outlineLevel="1">
       <c r="A10" s="72"/>
-      <c r="B10" s="140" t="s">
+      <c r="B10" s="164" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="149" t="s">
+      <c r="C10" s="172" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="141" t="s">
+      <c r="D10" s="144" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="141"/>
+      <c r="E10" s="144"/>
       <c r="F10" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="153" t="s">
+      <c r="G10" s="131" t="s">
         <v>96</v>
       </c>
-      <c r="H10" s="153"/>
-      <c r="I10" s="153"/>
+      <c r="H10" s="131"/>
+      <c r="I10" s="131"/>
       <c r="J10" s="74" t="s">
         <v>87</v>
       </c>
       <c r="K10" s="73" t="s">
         <v>99</v>
       </c>
-      <c r="L10" s="141">
+      <c r="L10" s="144">
         <v>5</v>
       </c>
-      <c r="M10" s="141"/>
-      <c r="N10" s="140" t="s">
+      <c r="M10" s="144"/>
+      <c r="N10" s="164" t="s">
         <v>43</v>
       </c>
-      <c r="O10" s="152" t="s">
+      <c r="O10" s="133" t="s">
         <v>92</v>
       </c>
       <c r="P10" s="75"/>
     </row>
-    <row r="11" spans="1:16" s="76" customFormat="1" ht="16.5" customHeight="1" outlineLevel="1">
+    <row r="11" spans="1:23" s="76" customFormat="1" ht="16.5" customHeight="1" outlineLevel="1">
       <c r="A11" s="72"/>
-      <c r="B11" s="140"/>
-      <c r="C11" s="150"/>
-      <c r="D11" s="141"/>
-      <c r="E11" s="141"/>
+      <c r="B11" s="164"/>
+      <c r="C11" s="173"/>
+      <c r="D11" s="144"/>
+      <c r="E11" s="144"/>
       <c r="F11" s="73"/>
-      <c r="G11" s="142" t="s">
+      <c r="G11" s="134" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="142"/>
-      <c r="I11" s="142"/>
+      <c r="H11" s="134"/>
+      <c r="I11" s="134"/>
       <c r="J11" s="74" t="s">
         <v>20</v>
       </c>
       <c r="K11" s="73"/>
-      <c r="L11" s="141"/>
-      <c r="M11" s="141"/>
-      <c r="N11" s="141"/>
-      <c r="O11" s="152"/>
+      <c r="L11" s="144"/>
+      <c r="M11" s="144"/>
+      <c r="N11" s="144"/>
+      <c r="O11" s="133"/>
       <c r="P11" s="75"/>
     </row>
-    <row r="12" spans="1:16" s="76" customFormat="1" ht="16.5" customHeight="1" outlineLevel="1">
+    <row r="12" spans="1:23" s="76" customFormat="1" ht="16.5" customHeight="1" outlineLevel="1">
       <c r="A12" s="72"/>
-      <c r="B12" s="140"/>
-      <c r="C12" s="151"/>
-      <c r="D12" s="141" t="s">
+      <c r="B12" s="164"/>
+      <c r="C12" s="174"/>
+      <c r="D12" s="144" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="141"/>
+      <c r="E12" s="144"/>
       <c r="F12" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="153" t="s">
+      <c r="G12" s="131" t="s">
         <v>96</v>
       </c>
-      <c r="H12" s="153"/>
-      <c r="I12" s="153"/>
+      <c r="H12" s="131"/>
+      <c r="I12" s="131"/>
       <c r="J12" s="74" t="str">
         <f>J10</f>
         <v>800+150mm</v>
@@ -3599,68 +3609,68 @@
       <c r="K12" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="L12" s="141">
+      <c r="L12" s="144">
         <v>3</v>
       </c>
-      <c r="M12" s="141"/>
-      <c r="N12" s="141"/>
-      <c r="O12" s="152"/>
+      <c r="M12" s="144"/>
+      <c r="N12" s="144"/>
+      <c r="O12" s="133"/>
       <c r="P12" s="75"/>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:23">
       <c r="A13" s="41"/>
       <c r="P13" s="5"/>
     </row>
-    <row r="14" spans="1:16" s="76" customFormat="1" ht="16.5" customHeight="1" outlineLevel="1">
+    <row r="14" spans="1:23" s="76" customFormat="1" ht="16.5" customHeight="1" outlineLevel="1">
       <c r="A14" s="72"/>
-      <c r="B14" s="140" t="s">
+      <c r="B14" s="164" t="s">
         <v>91</v>
       </c>
-      <c r="C14" s="140" t="s">
+      <c r="C14" s="164" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="141">
+      <c r="D14" s="144">
         <v>1</v>
       </c>
-      <c r="E14" s="141"/>
+      <c r="E14" s="144"/>
       <c r="F14" s="96" t="s">
         <v>64</v>
       </c>
-      <c r="G14" s="142" t="s">
+      <c r="G14" s="134" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="142"/>
-      <c r="I14" s="142"/>
+      <c r="H14" s="134"/>
+      <c r="I14" s="134"/>
       <c r="J14" s="74" t="s">
         <v>89</v>
       </c>
       <c r="K14" s="96" t="s">
         <v>64</v>
       </c>
-      <c r="L14" s="146" t="s">
+      <c r="L14" s="168" t="s">
         <v>58</v>
       </c>
-      <c r="M14" s="147"/>
+      <c r="M14" s="169"/>
       <c r="N14" s="92"/>
       <c r="O14" s="93"/>
       <c r="P14" s="75"/>
     </row>
-    <row r="15" spans="1:16" s="76" customFormat="1" ht="16.5" customHeight="1" outlineLevel="1">
+    <row r="15" spans="1:23" s="76" customFormat="1" ht="16.5" customHeight="1" outlineLevel="1">
       <c r="A15" s="72"/>
-      <c r="B15" s="140"/>
-      <c r="C15" s="140"/>
-      <c r="D15" s="141">
+      <c r="B15" s="164"/>
+      <c r="C15" s="164"/>
+      <c r="D15" s="144">
         <v>2</v>
       </c>
-      <c r="E15" s="141"/>
+      <c r="E15" s="144"/>
       <c r="F15" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="G15" s="142" t="s">
+      <c r="G15" s="134" t="s">
         <v>38</v>
       </c>
-      <c r="H15" s="142"/>
-      <c r="I15" s="142"/>
+      <c r="H15" s="134"/>
+      <c r="I15" s="134"/>
       <c r="J15" s="74" t="str">
         <f>J14</f>
         <v>350mm</v>
@@ -3668,30 +3678,30 @@
       <c r="K15" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="L15" s="146" t="s">
+      <c r="L15" s="168" t="s">
         <v>59</v>
       </c>
-      <c r="M15" s="147"/>
+      <c r="M15" s="169"/>
       <c r="N15" s="92"/>
       <c r="O15" s="93"/>
       <c r="P15" s="75"/>
     </row>
-    <row r="16" spans="1:16" s="76" customFormat="1" ht="16.5" customHeight="1" outlineLevel="1">
+    <row r="16" spans="1:23" s="76" customFormat="1" ht="16.5" customHeight="1" outlineLevel="1">
       <c r="A16" s="72"/>
-      <c r="B16" s="140"/>
-      <c r="C16" s="140"/>
-      <c r="D16" s="141">
+      <c r="B16" s="164"/>
+      <c r="C16" s="164"/>
+      <c r="D16" s="144">
         <v>3</v>
       </c>
-      <c r="E16" s="141"/>
+      <c r="E16" s="144"/>
       <c r="F16" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="G16" s="142" t="s">
+      <c r="G16" s="134" t="s">
         <v>38</v>
       </c>
-      <c r="H16" s="142"/>
-      <c r="I16" s="142"/>
+      <c r="H16" s="134"/>
+      <c r="I16" s="134"/>
       <c r="J16" s="74" t="str">
         <f>J14</f>
         <v>350mm</v>
@@ -3699,40 +3709,40 @@
       <c r="K16" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="L16" s="146" t="s">
+      <c r="L16" s="168" t="s">
         <v>60</v>
       </c>
-      <c r="M16" s="147"/>
+      <c r="M16" s="169"/>
       <c r="N16" s="92"/>
       <c r="O16" s="93"/>
       <c r="P16" s="75"/>
     </row>
     <row r="17" spans="1:16" s="76" customFormat="1" ht="16.5" customHeight="1" outlineLevel="1">
       <c r="A17" s="72"/>
-      <c r="B17" s="140"/>
-      <c r="C17" s="140"/>
-      <c r="D17" s="141">
+      <c r="B17" s="164"/>
+      <c r="C17" s="164"/>
+      <c r="D17" s="144">
         <v>4</v>
       </c>
-      <c r="E17" s="141"/>
+      <c r="E17" s="144"/>
       <c r="F17" s="96" t="s">
         <v>67</v>
       </c>
-      <c r="G17" s="142" t="s">
+      <c r="G17" s="134" t="s">
         <v>38</v>
       </c>
-      <c r="H17" s="142"/>
-      <c r="I17" s="142"/>
+      <c r="H17" s="134"/>
+      <c r="I17" s="134"/>
       <c r="J17" s="107" t="s">
         <v>88</v>
       </c>
       <c r="K17" s="102" t="s">
         <v>67</v>
       </c>
-      <c r="L17" s="148">
+      <c r="L17" s="170">
         <v>2</v>
       </c>
-      <c r="M17" s="148"/>
+      <c r="M17" s="170"/>
       <c r="N17" s="103" t="s">
         <v>63</v>
       </c>
@@ -3743,20 +3753,20 @@
     </row>
     <row r="18" spans="1:16" s="76" customFormat="1" ht="16.5" customHeight="1" outlineLevel="1">
       <c r="A18" s="72"/>
-      <c r="B18" s="140"/>
-      <c r="C18" s="140"/>
-      <c r="D18" s="141">
+      <c r="B18" s="164"/>
+      <c r="C18" s="164"/>
+      <c r="D18" s="144">
         <v>5</v>
       </c>
-      <c r="E18" s="141"/>
+      <c r="E18" s="144"/>
       <c r="F18" s="94" t="s">
         <v>68</v>
       </c>
-      <c r="G18" s="142" t="s">
+      <c r="G18" s="134" t="s">
         <v>38</v>
       </c>
-      <c r="H18" s="142"/>
-      <c r="I18" s="142"/>
+      <c r="H18" s="134"/>
+      <c r="I18" s="134"/>
       <c r="J18" s="74" t="str">
         <f>J14</f>
         <v>350mm</v>
@@ -3764,30 +3774,30 @@
       <c r="K18" s="94" t="s">
         <v>68</v>
       </c>
-      <c r="L18" s="141" t="s">
+      <c r="L18" s="144" t="s">
         <v>58</v>
       </c>
-      <c r="M18" s="141"/>
+      <c r="M18" s="144"/>
       <c r="N18" s="92"/>
       <c r="O18" s="93"/>
       <c r="P18" s="75"/>
     </row>
     <row r="19" spans="1:16" s="76" customFormat="1" ht="16.5" customHeight="1" outlineLevel="1">
       <c r="A19" s="72"/>
-      <c r="B19" s="140"/>
-      <c r="C19" s="140"/>
-      <c r="D19" s="141">
+      <c r="B19" s="164"/>
+      <c r="C19" s="164"/>
+      <c r="D19" s="144">
         <v>6</v>
       </c>
-      <c r="E19" s="141"/>
+      <c r="E19" s="144"/>
       <c r="F19" s="95" t="s">
         <v>69</v>
       </c>
-      <c r="G19" s="142" t="s">
+      <c r="G19" s="134" t="s">
         <v>38</v>
       </c>
-      <c r="H19" s="142"/>
-      <c r="I19" s="142"/>
+      <c r="H19" s="134"/>
+      <c r="I19" s="134"/>
       <c r="J19" s="74" t="str">
         <f>J14</f>
         <v>350mm</v>
@@ -3795,30 +3805,30 @@
       <c r="K19" s="95" t="s">
         <v>69</v>
       </c>
-      <c r="L19" s="141" t="s">
+      <c r="L19" s="144" t="s">
         <v>59</v>
       </c>
-      <c r="M19" s="141"/>
+      <c r="M19" s="144"/>
       <c r="N19" s="92"/>
       <c r="O19" s="93"/>
       <c r="P19" s="75"/>
     </row>
     <row r="20" spans="1:16" s="76" customFormat="1" ht="16.5" customHeight="1" outlineLevel="1">
       <c r="A20" s="72"/>
-      <c r="B20" s="140"/>
-      <c r="C20" s="140"/>
-      <c r="D20" s="141">
+      <c r="B20" s="164"/>
+      <c r="C20" s="164"/>
+      <c r="D20" s="144">
         <v>7</v>
       </c>
-      <c r="E20" s="141"/>
+      <c r="E20" s="144"/>
       <c r="F20" s="95" t="s">
         <v>70</v>
       </c>
-      <c r="G20" s="142" t="s">
+      <c r="G20" s="134" t="s">
         <v>38</v>
       </c>
-      <c r="H20" s="142"/>
-      <c r="I20" s="142"/>
+      <c r="H20" s="134"/>
+      <c r="I20" s="134"/>
       <c r="J20" s="74" t="str">
         <f>J14</f>
         <v>350mm</v>
@@ -3826,40 +3836,40 @@
       <c r="K20" s="95" t="s">
         <v>70</v>
       </c>
-      <c r="L20" s="141" t="s">
+      <c r="L20" s="144" t="s">
         <v>60</v>
       </c>
-      <c r="M20" s="141"/>
+      <c r="M20" s="144"/>
       <c r="N20" s="92"/>
       <c r="O20" s="93"/>
       <c r="P20" s="75"/>
     </row>
     <row r="21" spans="1:16" s="76" customFormat="1" ht="16.5" customHeight="1" outlineLevel="1">
       <c r="A21" s="72"/>
-      <c r="B21" s="140"/>
-      <c r="C21" s="140"/>
-      <c r="D21" s="141">
+      <c r="B21" s="164"/>
+      <c r="C21" s="164"/>
+      <c r="D21" s="144">
         <v>8</v>
       </c>
-      <c r="E21" s="141"/>
+      <c r="E21" s="144"/>
       <c r="F21" s="95" t="s">
         <v>71</v>
       </c>
-      <c r="G21" s="142" t="s">
+      <c r="G21" s="134" t="s">
         <v>38</v>
       </c>
-      <c r="H21" s="142"/>
-      <c r="I21" s="142"/>
+      <c r="H21" s="134"/>
+      <c r="I21" s="134"/>
       <c r="J21" s="107" t="s">
         <v>88</v>
       </c>
       <c r="K21" s="105" t="s">
         <v>71</v>
       </c>
-      <c r="L21" s="148">
+      <c r="L21" s="170">
         <v>1</v>
       </c>
-      <c r="M21" s="148"/>
+      <c r="M21" s="170"/>
       <c r="N21" s="103" t="s">
         <v>63</v>
       </c>
@@ -3874,58 +3884,58 @@
     </row>
     <row r="23" spans="1:16" s="76" customFormat="1" ht="16.5" customHeight="1" outlineLevel="1">
       <c r="A23" s="72"/>
-      <c r="B23" s="140" t="s">
+      <c r="B23" s="164" t="s">
         <v>94</v>
       </c>
-      <c r="C23" s="140" t="s">
+      <c r="C23" s="164" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="141">
+      <c r="D23" s="144">
         <v>1</v>
       </c>
-      <c r="E23" s="141"/>
+      <c r="E23" s="144"/>
       <c r="F23" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="G23" s="142" t="s">
+      <c r="G23" s="134" t="s">
         <v>38</v>
       </c>
-      <c r="H23" s="142"/>
-      <c r="I23" s="142"/>
+      <c r="H23" s="134"/>
+      <c r="I23" s="134"/>
       <c r="J23" s="74" t="s">
         <v>88</v>
       </c>
       <c r="K23" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="L23" s="141">
+      <c r="L23" s="144">
         <v>1</v>
       </c>
-      <c r="M23" s="141"/>
-      <c r="N23" s="140" t="s">
+      <c r="M23" s="144"/>
+      <c r="N23" s="164" t="s">
         <v>74</v>
       </c>
-      <c r="O23" s="140" t="s">
+      <c r="O23" s="164" t="s">
         <v>95</v>
       </c>
       <c r="P23" s="75"/>
     </row>
     <row r="24" spans="1:16" s="76" customFormat="1" ht="16.5" customHeight="1" outlineLevel="1">
       <c r="A24" s="72"/>
-      <c r="B24" s="140"/>
-      <c r="C24" s="140"/>
-      <c r="D24" s="141">
+      <c r="B24" s="164"/>
+      <c r="C24" s="164"/>
+      <c r="D24" s="144">
         <v>2</v>
       </c>
-      <c r="E24" s="141"/>
+      <c r="E24" s="144"/>
       <c r="F24" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="G24" s="142" t="s">
+      <c r="G24" s="134" t="s">
         <v>38</v>
       </c>
-      <c r="H24" s="142"/>
-      <c r="I24" s="142"/>
+      <c r="H24" s="134"/>
+      <c r="I24" s="134"/>
       <c r="J24" s="74" t="str">
         <f>J23</f>
         <v>250mm</v>
@@ -3933,12 +3943,12 @@
       <c r="K24" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="L24" s="141">
+      <c r="L24" s="144">
         <v>2</v>
       </c>
-      <c r="M24" s="141"/>
-      <c r="N24" s="140"/>
-      <c r="O24" s="140"/>
+      <c r="M24" s="144"/>
+      <c r="N24" s="164"/>
+      <c r="O24" s="164"/>
       <c r="P24" s="75"/>
     </row>
     <row r="25" spans="1:16">
@@ -3958,10 +3968,10 @@
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
-      <c r="G27" s="157"/>
-      <c r="H27" s="157"/>
-      <c r="I27" s="157"/>
-      <c r="J27" s="157"/>
+      <c r="G27" s="148"/>
+      <c r="H27" s="148"/>
+      <c r="I27" s="148"/>
+      <c r="J27" s="148"/>
       <c r="K27" s="3"/>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
@@ -3973,22 +3983,22 @@
       <c r="A28" s="41"/>
       <c r="B28" s="17"/>
       <c r="C28" s="3"/>
-      <c r="D28" s="161" t="str">
+      <c r="D28" s="152" t="str">
         <f>B5</f>
         <v>HARTING(통신)
 21 03 8822405</v>
       </c>
       <c r="E28" s="36"/>
       <c r="F28" s="10"/>
-      <c r="G28" s="164"/>
-      <c r="H28" s="167" t="s">
+      <c r="G28" s="155"/>
+      <c r="H28" s="158" t="s">
         <v>37</v>
       </c>
-      <c r="I28" s="167"/>
-      <c r="J28" s="154"/>
+      <c r="I28" s="158"/>
+      <c r="J28" s="145"/>
       <c r="K28" s="23"/>
       <c r="L28" s="11"/>
-      <c r="M28" s="170" t="str">
+      <c r="M28" s="161" t="str">
         <f>O5</f>
         <v>Main-PCB(J19)
 MOLEX
@@ -4002,7 +4012,7 @@
       <c r="A29" s="41"/>
       <c r="B29" s="17"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="162"/>
+      <c r="D29" s="153"/>
       <c r="E29" s="37">
         <v>1</v>
       </c>
@@ -4010,10 +4020,10 @@
         <f>F5</f>
         <v>0</v>
       </c>
-      <c r="G29" s="165"/>
-      <c r="H29" s="168"/>
-      <c r="I29" s="168"/>
-      <c r="J29" s="155"/>
+      <c r="G29" s="156"/>
+      <c r="H29" s="159"/>
+      <c r="I29" s="159"/>
+      <c r="J29" s="146"/>
       <c r="K29" s="115" t="str">
         <f>K5</f>
         <v>4 / TX+</v>
@@ -4021,16 +4031,16 @@
       <c r="L29" s="39">
         <v>4</v>
       </c>
-      <c r="M29" s="171"/>
+      <c r="M29" s="162"/>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
       <c r="P29" s="9"/>
     </row>
     <row r="30" spans="1:16" s="8" customFormat="1" ht="16.5" customHeight="1">
       <c r="A30" s="41"/>
-      <c r="B30" s="159"/>
-      <c r="C30" s="160"/>
-      <c r="D30" s="162"/>
+      <c r="B30" s="150"/>
+      <c r="C30" s="151"/>
+      <c r="D30" s="153"/>
       <c r="E30" s="37">
         <v>3</v>
       </c>
@@ -4038,10 +4048,10 @@
         <f t="shared" ref="F30:F32" si="0">F6</f>
         <v>0</v>
       </c>
-      <c r="G30" s="165"/>
-      <c r="H30" s="168"/>
-      <c r="I30" s="168"/>
-      <c r="J30" s="155"/>
+      <c r="G30" s="156"/>
+      <c r="H30" s="159"/>
+      <c r="I30" s="159"/>
+      <c r="J30" s="146"/>
       <c r="K30" s="32" t="str">
         <f t="shared" ref="K30:K32" si="1">K6</f>
         <v>3 / TX-</v>
@@ -4049,16 +4059,16 @@
       <c r="L30" s="39">
         <v>3</v>
       </c>
-      <c r="M30" s="171"/>
+      <c r="M30" s="162"/>
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
       <c r="P30" s="9"/>
     </row>
     <row r="31" spans="1:16" s="8" customFormat="1" ht="16.5" customHeight="1">
       <c r="A31" s="41"/>
-      <c r="B31" s="159"/>
-      <c r="C31" s="160"/>
-      <c r="D31" s="162"/>
+      <c r="B31" s="150"/>
+      <c r="C31" s="151"/>
+      <c r="D31" s="153"/>
       <c r="E31" s="37">
         <v>2</v>
       </c>
@@ -4066,10 +4076,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G31" s="165"/>
-      <c r="H31" s="168"/>
-      <c r="I31" s="168"/>
-      <c r="J31" s="155"/>
+      <c r="G31" s="156"/>
+      <c r="H31" s="159"/>
+      <c r="I31" s="159"/>
+      <c r="J31" s="146"/>
       <c r="K31" s="114" t="str">
         <f t="shared" si="1"/>
         <v>2 / RX+</v>
@@ -4077,7 +4087,7 @@
       <c r="L31" s="39">
         <v>2</v>
       </c>
-      <c r="M31" s="171"/>
+      <c r="M31" s="162"/>
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
       <c r="P31" s="9"/>
@@ -4086,7 +4096,7 @@
       <c r="A32" s="41"/>
       <c r="B32" s="17"/>
       <c r="C32" s="3"/>
-      <c r="D32" s="162"/>
+      <c r="D32" s="153"/>
       <c r="E32" s="37">
         <v>4</v>
       </c>
@@ -4094,10 +4104,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G32" s="165"/>
-      <c r="H32" s="168"/>
-      <c r="I32" s="168"/>
-      <c r="J32" s="155"/>
+      <c r="G32" s="156"/>
+      <c r="H32" s="159"/>
+      <c r="I32" s="159"/>
+      <c r="J32" s="146"/>
       <c r="K32" s="71" t="str">
         <f t="shared" si="1"/>
         <v>1 / RX-</v>
@@ -4105,7 +4115,7 @@
       <c r="L32" s="39">
         <v>1</v>
       </c>
-      <c r="M32" s="171"/>
+      <c r="M32" s="162"/>
       <c r="N32" s="4"/>
       <c r="O32" s="4"/>
       <c r="P32" s="9"/>
@@ -4114,31 +4124,31 @@
       <c r="A33" s="41"/>
       <c r="B33" s="17"/>
       <c r="C33" s="3"/>
-      <c r="D33" s="163"/>
+      <c r="D33" s="154"/>
       <c r="E33" s="38"/>
       <c r="F33" s="17"/>
-      <c r="G33" s="166"/>
-      <c r="H33" s="169"/>
-      <c r="I33" s="169"/>
-      <c r="J33" s="156"/>
+      <c r="G33" s="157"/>
+      <c r="H33" s="160"/>
+      <c r="I33" s="160"/>
+      <c r="J33" s="147"/>
       <c r="K33" s="17"/>
       <c r="L33" s="12"/>
-      <c r="M33" s="172"/>
+      <c r="M33" s="163"/>
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
       <c r="P33" s="9"/>
     </row>
     <row r="34" spans="1:16">
       <c r="A34" s="41"/>
-      <c r="F34" s="158" t="str">
+      <c r="F34" s="149" t="str">
         <f>J5</f>
         <v>800+350mm</v>
       </c>
-      <c r="G34" s="158"/>
-      <c r="H34" s="158"/>
-      <c r="I34" s="158"/>
-      <c r="J34" s="158"/>
-      <c r="K34" s="158"/>
+      <c r="G34" s="149"/>
+      <c r="H34" s="149"/>
+      <c r="I34" s="149"/>
+      <c r="J34" s="149"/>
+      <c r="K34" s="149"/>
       <c r="P34" s="5"/>
     </row>
     <row r="35" spans="1:16" ht="18" thickBot="1">
@@ -4149,22 +4159,22 @@
       <c r="A36" s="72"/>
       <c r="B36" s="77"/>
       <c r="C36" s="78"/>
-      <c r="D36" s="125" t="str">
+      <c r="D36" s="175" t="str">
         <f>B10</f>
         <v>WAGO(전원)
 770-213</v>
       </c>
       <c r="E36" s="79"/>
       <c r="F36" s="80"/>
-      <c r="G36" s="128"/>
-      <c r="H36" s="131" t="s">
+      <c r="G36" s="178"/>
+      <c r="H36" s="181" t="s">
         <v>37</v>
       </c>
-      <c r="I36" s="131"/>
-      <c r="J36" s="116"/>
+      <c r="I36" s="181"/>
+      <c r="J36" s="184"/>
       <c r="K36" s="81"/>
       <c r="L36" s="82"/>
-      <c r="M36" s="136" t="str">
+      <c r="M36" s="139" t="str">
         <f>O10</f>
         <v>POWER-PCB(CON1)
 YEONHO
@@ -4178,7 +4188,7 @@
       <c r="A37" s="72"/>
       <c r="B37" s="77"/>
       <c r="C37" s="78"/>
-      <c r="D37" s="126"/>
+      <c r="D37" s="176"/>
       <c r="E37" s="85" t="s">
         <v>35</v>
       </c>
@@ -4186,10 +4196,10 @@
         <f>F10</f>
         <v xml:space="preserve">L/DC 110V </v>
       </c>
-      <c r="G37" s="129"/>
-      <c r="H37" s="132"/>
-      <c r="I37" s="132"/>
-      <c r="J37" s="117"/>
+      <c r="G37" s="179"/>
+      <c r="H37" s="182"/>
+      <c r="I37" s="182"/>
+      <c r="J37" s="185"/>
       <c r="K37" s="97" t="str">
         <f>K10</f>
         <v>5 / DC 110V</v>
@@ -4197,34 +4207,34 @@
       <c r="L37" s="111">
         <v>5</v>
       </c>
-      <c r="M37" s="137"/>
+      <c r="M37" s="140"/>
       <c r="N37" s="83"/>
       <c r="O37" s="83"/>
       <c r="P37" s="24"/>
     </row>
     <row r="38" spans="1:16" s="25" customFormat="1" ht="16.5" customHeight="1">
       <c r="A38" s="72"/>
-      <c r="B38" s="134"/>
-      <c r="C38" s="135"/>
-      <c r="D38" s="126"/>
+      <c r="B38" s="142"/>
+      <c r="C38" s="143"/>
+      <c r="D38" s="176"/>
       <c r="E38" s="85"/>
       <c r="F38" s="86"/>
-      <c r="G38" s="129"/>
-      <c r="H38" s="132"/>
-      <c r="I38" s="132"/>
-      <c r="J38" s="117"/>
+      <c r="G38" s="179"/>
+      <c r="H38" s="182"/>
+      <c r="I38" s="182"/>
+      <c r="J38" s="185"/>
       <c r="K38" s="86"/>
       <c r="L38" s="84"/>
-      <c r="M38" s="137"/>
+      <c r="M38" s="140"/>
       <c r="N38" s="83"/>
       <c r="O38" s="83"/>
       <c r="P38" s="24"/>
     </row>
     <row r="39" spans="1:16" s="25" customFormat="1" ht="16.5" customHeight="1">
       <c r="A39" s="72"/>
-      <c r="B39" s="134"/>
-      <c r="C39" s="135"/>
-      <c r="D39" s="126"/>
+      <c r="B39" s="142"/>
+      <c r="C39" s="143"/>
+      <c r="D39" s="176"/>
       <c r="E39" s="85" t="s">
         <v>36</v>
       </c>
@@ -4232,10 +4242,10 @@
         <f>F12</f>
         <v xml:space="preserve">N/DC GND </v>
       </c>
-      <c r="G39" s="129"/>
-      <c r="H39" s="132"/>
-      <c r="I39" s="132"/>
-      <c r="J39" s="117"/>
+      <c r="G39" s="179"/>
+      <c r="H39" s="182"/>
+      <c r="I39" s="182"/>
+      <c r="J39" s="185"/>
       <c r="K39" s="86" t="str">
         <f>K12</f>
         <v>3 / DC GND</v>
@@ -4243,7 +4253,7 @@
       <c r="L39" s="84">
         <v>3</v>
       </c>
-      <c r="M39" s="137"/>
+      <c r="M39" s="140"/>
       <c r="N39" s="83"/>
       <c r="O39" s="83"/>
       <c r="P39" s="24"/>
@@ -4252,16 +4262,16 @@
       <c r="A40" s="72"/>
       <c r="B40" s="77"/>
       <c r="C40" s="78"/>
-      <c r="D40" s="127"/>
+      <c r="D40" s="177"/>
       <c r="E40" s="87"/>
       <c r="F40" s="88"/>
-      <c r="G40" s="130"/>
-      <c r="H40" s="133"/>
-      <c r="I40" s="133"/>
-      <c r="J40" s="118"/>
+      <c r="G40" s="180"/>
+      <c r="H40" s="183"/>
+      <c r="I40" s="183"/>
+      <c r="J40" s="186"/>
       <c r="K40" s="88"/>
       <c r="L40" s="89"/>
-      <c r="M40" s="138"/>
+      <c r="M40" s="141"/>
       <c r="N40" s="83"/>
       <c r="O40" s="83"/>
       <c r="P40" s="24"/>
@@ -4272,15 +4282,15 @@
       <c r="C41" s="78"/>
       <c r="D41" s="78"/>
       <c r="E41" s="78"/>
-      <c r="F41" s="119" t="str">
+      <c r="F41" s="171" t="str">
         <f>J10</f>
         <v>800+150mm</v>
       </c>
-      <c r="G41" s="119"/>
-      <c r="H41" s="119"/>
-      <c r="I41" s="119"/>
-      <c r="J41" s="119"/>
-      <c r="K41" s="119"/>
+      <c r="G41" s="171"/>
+      <c r="H41" s="171"/>
+      <c r="I41" s="171"/>
+      <c r="J41" s="171"/>
+      <c r="K41" s="171"/>
       <c r="L41" s="83"/>
       <c r="M41" s="83"/>
       <c r="N41" s="83"/>
@@ -4327,7 +4337,7 @@
       <c r="A44" s="72"/>
       <c r="B44" s="77"/>
       <c r="C44" s="78"/>
-      <c r="D44" s="125" t="str">
+      <c r="D44" s="175" t="str">
         <f>B14</f>
         <v>POWER-PCB(CON3)
 YHEOHO
@@ -4335,10 +4345,10 @@
       </c>
       <c r="E44" s="79"/>
       <c r="F44" s="80"/>
-      <c r="G44" s="128"/>
-      <c r="H44" s="131"/>
-      <c r="I44" s="131"/>
-      <c r="J44" s="116"/>
+      <c r="G44" s="178"/>
+      <c r="H44" s="181"/>
+      <c r="I44" s="181"/>
+      <c r="J44" s="184"/>
       <c r="K44" s="81"/>
       <c r="L44" s="82"/>
       <c r="M44" s="98"/>
@@ -4350,7 +4360,7 @@
       <c r="A45" s="72"/>
       <c r="B45" s="77"/>
       <c r="C45" s="78"/>
-      <c r="D45" s="126"/>
+      <c r="D45" s="176"/>
       <c r="E45" s="85">
         <v>1</v>
       </c>
@@ -4358,14 +4368,14 @@
         <f>F14</f>
         <v>1 / 5V-</v>
       </c>
-      <c r="G45" s="129"/>
-      <c r="H45" s="132"/>
-      <c r="I45" s="132"/>
-      <c r="J45" s="117"/>
+      <c r="G45" s="179"/>
+      <c r="H45" s="182"/>
+      <c r="I45" s="182"/>
+      <c r="J45" s="185"/>
       <c r="K45" s="86" t="s">
         <v>78</v>
       </c>
-      <c r="L45" s="120" t="s">
+      <c r="L45" s="187" t="s">
         <v>76</v>
       </c>
       <c r="M45" s="99" t="s">
@@ -4377,9 +4387,9 @@
     </row>
     <row r="46" spans="1:16" s="25" customFormat="1" ht="16.5" customHeight="1">
       <c r="A46" s="72"/>
-      <c r="B46" s="134"/>
-      <c r="C46" s="135"/>
-      <c r="D46" s="126"/>
+      <c r="B46" s="142"/>
+      <c r="C46" s="143"/>
+      <c r="D46" s="176"/>
       <c r="E46" s="85">
         <v>2</v>
       </c>
@@ -4387,14 +4397,14 @@
         <f t="shared" ref="F46:F52" si="2">F15</f>
         <v>2 /  5V-</v>
       </c>
-      <c r="G46" s="129"/>
-      <c r="H46" s="132"/>
-      <c r="I46" s="132"/>
-      <c r="J46" s="117"/>
+      <c r="G46" s="179"/>
+      <c r="H46" s="182"/>
+      <c r="I46" s="182"/>
+      <c r="J46" s="185"/>
       <c r="K46" s="86" t="s">
         <v>78</v>
       </c>
-      <c r="L46" s="120"/>
+      <c r="L46" s="187"/>
       <c r="M46" s="99" t="s">
         <v>84</v>
       </c>
@@ -4404,9 +4414,9 @@
     </row>
     <row r="47" spans="1:16" s="25" customFormat="1" ht="16.5" customHeight="1">
       <c r="A47" s="72"/>
-      <c r="B47" s="134"/>
-      <c r="C47" s="135"/>
-      <c r="D47" s="126"/>
+      <c r="B47" s="142"/>
+      <c r="C47" s="143"/>
+      <c r="D47" s="176"/>
       <c r="E47" s="85">
         <v>3</v>
       </c>
@@ -4414,14 +4424,14 @@
         <f t="shared" si="2"/>
         <v>3 / 5V-</v>
       </c>
-      <c r="G47" s="129"/>
-      <c r="H47" s="132"/>
-      <c r="I47" s="132"/>
-      <c r="J47" s="117"/>
+      <c r="G47" s="179"/>
+      <c r="H47" s="182"/>
+      <c r="I47" s="182"/>
+      <c r="J47" s="185"/>
       <c r="K47" s="86" t="s">
         <v>78</v>
       </c>
-      <c r="L47" s="120"/>
+      <c r="L47" s="187"/>
       <c r="M47" s="99" t="s">
         <v>85</v>
       </c>
@@ -4431,9 +4441,9 @@
     </row>
     <row r="48" spans="1:16" s="25" customFormat="1" ht="16.5" customHeight="1">
       <c r="A48" s="72"/>
-      <c r="B48" s="134"/>
-      <c r="C48" s="135"/>
-      <c r="D48" s="126"/>
+      <c r="B48" s="142"/>
+      <c r="C48" s="143"/>
+      <c r="D48" s="176"/>
       <c r="E48" s="85">
         <v>4</v>
       </c>
@@ -4441,10 +4451,10 @@
         <f t="shared" si="2"/>
         <v>4 / 5V-</v>
       </c>
-      <c r="G48" s="129"/>
-      <c r="H48" s="132"/>
-      <c r="I48" s="132"/>
-      <c r="J48" s="117"/>
+      <c r="G48" s="179"/>
+      <c r="H48" s="182"/>
+      <c r="I48" s="182"/>
+      <c r="J48" s="185"/>
       <c r="K48" s="108" t="s">
         <v>79</v>
       </c>
@@ -4460,9 +4470,9 @@
     </row>
     <row r="49" spans="1:16" s="25" customFormat="1" ht="16.5" customHeight="1">
       <c r="A49" s="72"/>
-      <c r="B49" s="134"/>
-      <c r="C49" s="135"/>
-      <c r="D49" s="126"/>
+      <c r="B49" s="142"/>
+      <c r="C49" s="143"/>
+      <c r="D49" s="176"/>
       <c r="E49" s="85">
         <v>5</v>
       </c>
@@ -4470,14 +4480,14 @@
         <f t="shared" si="2"/>
         <v>5 / 5V+</v>
       </c>
-      <c r="G49" s="129"/>
-      <c r="H49" s="132"/>
-      <c r="I49" s="132"/>
-      <c r="J49" s="117"/>
+      <c r="G49" s="179"/>
+      <c r="H49" s="182"/>
+      <c r="I49" s="182"/>
+      <c r="J49" s="185"/>
       <c r="K49" s="101" t="s">
         <v>77</v>
       </c>
-      <c r="L49" s="120" t="s">
+      <c r="L49" s="187" t="s">
         <v>75</v>
       </c>
       <c r="M49" s="99" t="s">
@@ -4491,7 +4501,7 @@
       <c r="A50" s="72"/>
       <c r="B50" s="77"/>
       <c r="C50" s="78"/>
-      <c r="D50" s="126"/>
+      <c r="D50" s="176"/>
       <c r="E50" s="85">
         <v>6</v>
       </c>
@@ -4499,14 +4509,14 @@
         <f t="shared" si="2"/>
         <v>6 / 5V+</v>
       </c>
-      <c r="G50" s="129"/>
-      <c r="H50" s="132"/>
-      <c r="I50" s="132"/>
-      <c r="J50" s="117"/>
+      <c r="G50" s="179"/>
+      <c r="H50" s="182"/>
+      <c r="I50" s="182"/>
+      <c r="J50" s="185"/>
       <c r="K50" s="101" t="s">
         <v>77</v>
       </c>
-      <c r="L50" s="120"/>
+      <c r="L50" s="187"/>
       <c r="M50" s="99" t="s">
         <v>84</v>
       </c>
@@ -4518,7 +4528,7 @@
       <c r="A51" s="72"/>
       <c r="B51" s="90"/>
       <c r="C51" s="90"/>
-      <c r="D51" s="126"/>
+      <c r="D51" s="176"/>
       <c r="E51" s="85">
         <v>7</v>
       </c>
@@ -4526,14 +4536,14 @@
         <f t="shared" si="2"/>
         <v>7 / 5V+</v>
       </c>
-      <c r="G51" s="129"/>
-      <c r="H51" s="132"/>
-      <c r="I51" s="132"/>
-      <c r="J51" s="117"/>
+      <c r="G51" s="179"/>
+      <c r="H51" s="182"/>
+      <c r="I51" s="182"/>
+      <c r="J51" s="185"/>
       <c r="K51" s="101" t="s">
         <v>77</v>
       </c>
-      <c r="L51" s="120"/>
+      <c r="L51" s="187"/>
       <c r="M51" s="99" t="s">
         <v>85</v>
       </c>
@@ -4545,7 +4555,7 @@
       <c r="A52" s="72"/>
       <c r="B52" s="90"/>
       <c r="C52" s="90"/>
-      <c r="D52" s="126"/>
+      <c r="D52" s="176"/>
       <c r="E52" s="85">
         <v>8</v>
       </c>
@@ -4553,10 +4563,10 @@
         <f t="shared" si="2"/>
         <v>8 / 5V+</v>
       </c>
-      <c r="G52" s="129"/>
-      <c r="H52" s="132"/>
-      <c r="I52" s="132"/>
-      <c r="J52" s="117"/>
+      <c r="G52" s="179"/>
+      <c r="H52" s="182"/>
+      <c r="I52" s="182"/>
+      <c r="J52" s="185"/>
       <c r="K52" s="108" t="s">
         <v>57</v>
       </c>
@@ -4574,13 +4584,13 @@
       <c r="A53" s="72"/>
       <c r="B53" s="77"/>
       <c r="C53" s="78"/>
-      <c r="D53" s="127"/>
+      <c r="D53" s="177"/>
       <c r="E53" s="87"/>
       <c r="F53" s="88"/>
-      <c r="G53" s="130"/>
-      <c r="H53" s="133"/>
-      <c r="I53" s="133"/>
-      <c r="J53" s="118"/>
+      <c r="G53" s="180"/>
+      <c r="H53" s="183"/>
+      <c r="I53" s="183"/>
+      <c r="J53" s="186"/>
       <c r="K53" s="88"/>
       <c r="L53" s="89"/>
       <c r="M53" s="100"/>
@@ -4594,15 +4604,15 @@
       <c r="C54" s="78"/>
       <c r="D54" s="78"/>
       <c r="E54" s="78"/>
-      <c r="F54" s="119" t="str">
+      <c r="F54" s="171" t="str">
         <f>J14</f>
         <v>350mm</v>
       </c>
-      <c r="G54" s="119"/>
-      <c r="H54" s="119"/>
-      <c r="I54" s="119"/>
-      <c r="J54" s="119"/>
-      <c r="K54" s="119"/>
+      <c r="G54" s="171"/>
+      <c r="H54" s="171"/>
+      <c r="I54" s="171"/>
+      <c r="J54" s="171"/>
+      <c r="K54" s="171"/>
       <c r="L54" s="83"/>
       <c r="M54" s="83"/>
       <c r="N54" s="83"/>
@@ -4649,20 +4659,20 @@
       <c r="A57" s="72"/>
       <c r="B57" s="77"/>
       <c r="C57" s="78"/>
-      <c r="D57" s="125" t="str">
+      <c r="D57" s="175" t="str">
         <f>B23</f>
         <v>Main-PCB(J2) /MOLEX
 35155-0200</v>
       </c>
       <c r="E57" s="79"/>
       <c r="F57" s="80"/>
-      <c r="G57" s="128"/>
-      <c r="H57" s="131"/>
-      <c r="I57" s="131"/>
-      <c r="J57" s="116"/>
+      <c r="G57" s="178"/>
+      <c r="H57" s="181"/>
+      <c r="I57" s="181"/>
+      <c r="J57" s="184"/>
       <c r="K57" s="81"/>
       <c r="L57" s="82"/>
-      <c r="M57" s="136" t="str">
+      <c r="M57" s="139" t="str">
         <f>O23</f>
         <v>POWER-PCB(CON2) / MOLEX
 5051-02</v>
@@ -4675,7 +4685,7 @@
       <c r="A58" s="72"/>
       <c r="B58" s="77"/>
       <c r="C58" s="78"/>
-      <c r="D58" s="126"/>
+      <c r="D58" s="176"/>
       <c r="E58" s="85">
         <v>1</v>
       </c>
@@ -4683,10 +4693,10 @@
         <f>F23</f>
         <v>1 / RST</v>
       </c>
-      <c r="G58" s="129"/>
-      <c r="H58" s="132"/>
-      <c r="I58" s="132"/>
-      <c r="J58" s="117"/>
+      <c r="G58" s="179"/>
+      <c r="H58" s="182"/>
+      <c r="I58" s="182"/>
+      <c r="J58" s="185"/>
       <c r="K58" s="86" t="str">
         <f>K23</f>
         <v>1 / RST</v>
@@ -4694,16 +4704,16 @@
       <c r="L58" s="84">
         <v>1</v>
       </c>
-      <c r="M58" s="137"/>
+      <c r="M58" s="140"/>
       <c r="N58" s="83"/>
       <c r="O58" s="83"/>
       <c r="P58" s="24"/>
     </row>
     <row r="59" spans="1:16" s="25" customFormat="1" ht="16.5" customHeight="1">
       <c r="A59" s="72"/>
-      <c r="B59" s="134"/>
-      <c r="C59" s="135"/>
-      <c r="D59" s="126"/>
+      <c r="B59" s="142"/>
+      <c r="C59" s="143"/>
+      <c r="D59" s="176"/>
       <c r="E59" s="85">
         <v>2</v>
       </c>
@@ -4711,10 +4721,10 @@
         <f>F24</f>
         <v>2 / SGND</v>
       </c>
-      <c r="G59" s="129"/>
-      <c r="H59" s="132"/>
-      <c r="I59" s="132"/>
-      <c r="J59" s="117"/>
+      <c r="G59" s="179"/>
+      <c r="H59" s="182"/>
+      <c r="I59" s="182"/>
+      <c r="J59" s="185"/>
       <c r="K59" s="86" t="str">
         <f>K24</f>
         <v>2 / SGND</v>
@@ -4722,7 +4732,7 @@
       <c r="L59" s="84">
         <v>2</v>
       </c>
-      <c r="M59" s="137"/>
+      <c r="M59" s="140"/>
       <c r="N59" s="83"/>
       <c r="O59" s="83"/>
       <c r="P59" s="24"/>
@@ -4731,16 +4741,16 @@
       <c r="A60" s="72"/>
       <c r="B60" s="77"/>
       <c r="C60" s="78"/>
-      <c r="D60" s="127"/>
+      <c r="D60" s="177"/>
       <c r="E60" s="87"/>
       <c r="F60" s="88"/>
-      <c r="G60" s="130"/>
-      <c r="H60" s="133"/>
-      <c r="I60" s="133"/>
-      <c r="J60" s="118"/>
+      <c r="G60" s="180"/>
+      <c r="H60" s="183"/>
+      <c r="I60" s="183"/>
+      <c r="J60" s="186"/>
       <c r="K60" s="88"/>
       <c r="L60" s="89"/>
-      <c r="M60" s="138"/>
+      <c r="M60" s="141"/>
       <c r="N60" s="83"/>
       <c r="O60" s="83"/>
       <c r="P60" s="24"/>
@@ -4751,15 +4761,15 @@
       <c r="C61" s="78"/>
       <c r="D61" s="78"/>
       <c r="E61" s="78"/>
-      <c r="F61" s="119" t="str">
+      <c r="F61" s="171" t="str">
         <f>J23</f>
         <v>250mm</v>
       </c>
-      <c r="G61" s="119"/>
-      <c r="H61" s="119"/>
-      <c r="I61" s="119"/>
-      <c r="J61" s="119"/>
-      <c r="K61" s="119"/>
+      <c r="G61" s="171"/>
+      <c r="H61" s="171"/>
+      <c r="I61" s="171"/>
+      <c r="J61" s="171"/>
+      <c r="K61" s="171"/>
       <c r="L61" s="83"/>
       <c r="M61" s="83"/>
       <c r="N61" s="83"/>
@@ -4834,27 +4844,27 @@
       <c r="C66" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D66" s="139" t="s">
+      <c r="D66" s="129" t="s">
         <v>11</v>
       </c>
-      <c r="E66" s="139"/>
-      <c r="F66" s="139" t="s">
+      <c r="E66" s="129"/>
+      <c r="F66" s="129" t="s">
         <v>12</v>
       </c>
-      <c r="G66" s="139"/>
-      <c r="H66" s="139"/>
-      <c r="I66" s="139"/>
+      <c r="G66" s="129"/>
+      <c r="H66" s="129"/>
+      <c r="I66" s="129"/>
       <c r="J66" s="34" t="s">
         <v>13</v>
       </c>
       <c r="K66" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="L66" s="139" t="s">
+      <c r="L66" s="129" t="s">
         <v>15</v>
       </c>
-      <c r="M66" s="139"/>
-      <c r="N66" s="139"/>
+      <c r="M66" s="129"/>
+      <c r="N66" s="129"/>
       <c r="O66" s="34" t="s">
         <v>16</v>
       </c>
@@ -4869,27 +4879,27 @@
       <c r="C67" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D67" s="121" t="s">
+      <c r="D67" s="118" t="s">
         <v>25</v>
       </c>
-      <c r="E67" s="121"/>
-      <c r="F67" s="124" t="s">
+      <c r="E67" s="118"/>
+      <c r="F67" s="119" t="s">
         <v>27</v>
       </c>
-      <c r="G67" s="124"/>
-      <c r="H67" s="124"/>
-      <c r="I67" s="124"/>
+      <c r="G67" s="119"/>
+      <c r="H67" s="119"/>
+      <c r="I67" s="119"/>
       <c r="J67" s="27">
         <v>1</v>
       </c>
       <c r="K67" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="L67" s="123" t="s">
+      <c r="L67" s="117" t="s">
         <v>48</v>
       </c>
-      <c r="M67" s="123"/>
-      <c r="N67" s="123"/>
+      <c r="M67" s="117"/>
+      <c r="N67" s="117"/>
       <c r="O67" s="33" t="s">
         <v>28</v>
       </c>
@@ -4903,27 +4913,27 @@
       <c r="C68" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D68" s="121" t="s">
+      <c r="D68" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="E68" s="121"/>
-      <c r="F68" s="124" t="s">
+      <c r="E68" s="118"/>
+      <c r="F68" s="119" t="s">
         <v>27</v>
       </c>
-      <c r="G68" s="124"/>
-      <c r="H68" s="124"/>
-      <c r="I68" s="124"/>
+      <c r="G68" s="119"/>
+      <c r="H68" s="119"/>
+      <c r="I68" s="119"/>
       <c r="J68" s="27">
         <v>4</v>
       </c>
       <c r="K68" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="L68" s="123" t="s">
+      <c r="L68" s="117" t="s">
         <v>42</v>
       </c>
-      <c r="M68" s="123"/>
-      <c r="N68" s="123"/>
+      <c r="M68" s="117"/>
+      <c r="N68" s="117"/>
       <c r="O68" s="33"/>
       <c r="P68" s="9"/>
     </row>
@@ -4935,25 +4945,25 @@
       <c r="C69" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D69" s="121" t="s">
+      <c r="D69" s="118" t="s">
         <v>25</v>
       </c>
-      <c r="E69" s="121"/>
-      <c r="F69" s="122"/>
-      <c r="G69" s="122"/>
-      <c r="H69" s="122"/>
-      <c r="I69" s="122"/>
+      <c r="E69" s="118"/>
+      <c r="F69" s="116"/>
+      <c r="G69" s="116"/>
+      <c r="H69" s="116"/>
+      <c r="I69" s="116"/>
       <c r="J69" s="27">
         <v>1</v>
       </c>
       <c r="K69" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="L69" s="123" t="s">
+      <c r="L69" s="117" t="s">
         <v>49</v>
       </c>
-      <c r="M69" s="123"/>
-      <c r="N69" s="123"/>
+      <c r="M69" s="117"/>
+      <c r="N69" s="117"/>
       <c r="O69" s="27"/>
       <c r="P69" s="9"/>
     </row>
@@ -4965,25 +4975,25 @@
       <c r="C70" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D70" s="121" t="s">
+      <c r="D70" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="E70" s="121"/>
-      <c r="F70" s="122"/>
-      <c r="G70" s="122"/>
-      <c r="H70" s="122"/>
-      <c r="I70" s="122"/>
+      <c r="E70" s="118"/>
+      <c r="F70" s="116"/>
+      <c r="G70" s="116"/>
+      <c r="H70" s="116"/>
+      <c r="I70" s="116"/>
       <c r="J70" s="27">
         <v>6</v>
       </c>
       <c r="K70" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="L70" s="123" t="s">
+      <c r="L70" s="117" t="s">
         <v>54</v>
       </c>
-      <c r="M70" s="123"/>
-      <c r="N70" s="123"/>
+      <c r="M70" s="117"/>
+      <c r="N70" s="117"/>
       <c r="O70" s="27"/>
       <c r="P70" s="9"/>
     </row>
@@ -4995,25 +5005,25 @@
       <c r="C71" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="D71" s="121" t="s">
+      <c r="D71" s="118" t="s">
         <v>25</v>
       </c>
-      <c r="E71" s="121"/>
-      <c r="F71" s="122"/>
-      <c r="G71" s="122"/>
-      <c r="H71" s="122"/>
-      <c r="I71" s="122"/>
+      <c r="E71" s="118"/>
+      <c r="F71" s="116"/>
+      <c r="G71" s="116"/>
+      <c r="H71" s="116"/>
+      <c r="I71" s="116"/>
       <c r="J71" s="28">
         <v>1</v>
       </c>
       <c r="K71" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="L71" s="121" t="s">
+      <c r="L71" s="118" t="s">
         <v>51</v>
       </c>
-      <c r="M71" s="121"/>
-      <c r="N71" s="121"/>
+      <c r="M71" s="118"/>
+      <c r="N71" s="118"/>
       <c r="O71" s="28"/>
       <c r="P71" s="24"/>
     </row>
@@ -5025,25 +5035,25 @@
       <c r="C72" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D72" s="121" t="s">
+      <c r="D72" s="118" t="s">
         <v>25</v>
       </c>
-      <c r="E72" s="121"/>
-      <c r="F72" s="124"/>
-      <c r="G72" s="124"/>
-      <c r="H72" s="124"/>
-      <c r="I72" s="124"/>
+      <c r="E72" s="118"/>
+      <c r="F72" s="119"/>
+      <c r="G72" s="119"/>
+      <c r="H72" s="119"/>
+      <c r="I72" s="119"/>
       <c r="J72" s="27">
         <v>1</v>
       </c>
       <c r="K72" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="L72" s="123" t="s">
+      <c r="L72" s="117" t="s">
         <v>53</v>
       </c>
-      <c r="M72" s="123"/>
-      <c r="N72" s="123"/>
+      <c r="M72" s="117"/>
+      <c r="N72" s="117"/>
       <c r="O72" s="33"/>
       <c r="P72" s="9"/>
     </row>
@@ -5055,25 +5065,25 @@
       <c r="C73" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D73" s="121" t="s">
+      <c r="D73" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="E73" s="121"/>
-      <c r="F73" s="124"/>
-      <c r="G73" s="124"/>
-      <c r="H73" s="124"/>
-      <c r="I73" s="124"/>
+      <c r="E73" s="118"/>
+      <c r="F73" s="119"/>
+      <c r="G73" s="119"/>
+      <c r="H73" s="119"/>
+      <c r="I73" s="119"/>
       <c r="J73" s="27">
         <v>10</v>
       </c>
       <c r="K73" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="L73" s="123" t="s">
+      <c r="L73" s="117" t="s">
         <v>55</v>
       </c>
-      <c r="M73" s="123"/>
-      <c r="N73" s="123"/>
+      <c r="M73" s="117"/>
+      <c r="N73" s="117"/>
       <c r="O73" s="33"/>
       <c r="P73" s="9"/>
     </row>
@@ -5085,25 +5095,25 @@
       <c r="C74" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D74" s="121" t="s">
+      <c r="D74" s="118" t="s">
         <v>25</v>
       </c>
-      <c r="E74" s="121"/>
-      <c r="F74" s="122"/>
-      <c r="G74" s="122"/>
-      <c r="H74" s="122"/>
-      <c r="I74" s="122"/>
+      <c r="E74" s="118"/>
+      <c r="F74" s="116"/>
+      <c r="G74" s="116"/>
+      <c r="H74" s="116"/>
+      <c r="I74" s="116"/>
       <c r="J74" s="27">
         <v>1</v>
       </c>
       <c r="K74" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="L74" s="123" t="s">
+      <c r="L74" s="117" t="s">
         <v>80</v>
       </c>
-      <c r="M74" s="123"/>
-      <c r="N74" s="123"/>
+      <c r="M74" s="117"/>
+      <c r="N74" s="117"/>
       <c r="O74" s="27"/>
       <c r="P74" s="9"/>
     </row>
@@ -5115,25 +5125,25 @@
       <c r="C75" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="D75" s="121" t="s">
+      <c r="D75" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="E75" s="121"/>
-      <c r="F75" s="122"/>
-      <c r="G75" s="122"/>
-      <c r="H75" s="122"/>
-      <c r="I75" s="122"/>
+      <c r="E75" s="118"/>
+      <c r="F75" s="116"/>
+      <c r="G75" s="116"/>
+      <c r="H75" s="116"/>
+      <c r="I75" s="116"/>
       <c r="J75" s="28">
         <v>1</v>
       </c>
       <c r="K75" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="L75" s="121">
+      <c r="L75" s="118">
         <v>39012025</v>
       </c>
-      <c r="M75" s="121"/>
-      <c r="N75" s="121"/>
+      <c r="M75" s="118"/>
+      <c r="N75" s="118"/>
       <c r="O75" s="28"/>
       <c r="P75" s="24"/>
     </row>
@@ -5145,25 +5155,25 @@
       <c r="C76" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D76" s="121" t="s">
+      <c r="D76" s="118" t="s">
         <v>25</v>
       </c>
-      <c r="E76" s="121"/>
-      <c r="F76" s="122"/>
-      <c r="G76" s="122"/>
-      <c r="H76" s="122"/>
-      <c r="I76" s="122"/>
+      <c r="E76" s="118"/>
+      <c r="F76" s="116"/>
+      <c r="G76" s="116"/>
+      <c r="H76" s="116"/>
+      <c r="I76" s="116"/>
       <c r="J76" s="27">
         <v>2</v>
       </c>
       <c r="K76" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="L76" s="123" t="s">
+      <c r="L76" s="117" t="s">
         <v>63</v>
       </c>
-      <c r="M76" s="123"/>
-      <c r="N76" s="123"/>
+      <c r="M76" s="117"/>
+      <c r="N76" s="117"/>
       <c r="O76" s="27"/>
       <c r="P76" s="9"/>
     </row>
@@ -5175,25 +5185,25 @@
       <c r="C77" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D77" s="121" t="s">
+      <c r="D77" s="118" t="s">
         <v>25</v>
       </c>
-      <c r="E77" s="121"/>
-      <c r="F77" s="124"/>
-      <c r="G77" s="124"/>
-      <c r="H77" s="124"/>
-      <c r="I77" s="124"/>
+      <c r="E77" s="118"/>
+      <c r="F77" s="119"/>
+      <c r="G77" s="119"/>
+      <c r="H77" s="119"/>
+      <c r="I77" s="119"/>
       <c r="J77" s="27">
         <v>1</v>
       </c>
       <c r="K77" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="L77" s="123" t="s">
+      <c r="L77" s="117" t="s">
         <v>81</v>
       </c>
-      <c r="M77" s="123"/>
-      <c r="N77" s="123"/>
+      <c r="M77" s="117"/>
+      <c r="N77" s="117"/>
       <c r="O77" s="33"/>
       <c r="P77" s="9"/>
     </row>
@@ -5205,25 +5215,25 @@
       <c r="C78" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D78" s="121" t="s">
+      <c r="D78" s="118" t="s">
         <v>25</v>
       </c>
-      <c r="E78" s="121"/>
-      <c r="F78" s="122"/>
-      <c r="G78" s="122"/>
-      <c r="H78" s="122"/>
-      <c r="I78" s="122"/>
+      <c r="E78" s="118"/>
+      <c r="F78" s="116"/>
+      <c r="G78" s="116"/>
+      <c r="H78" s="116"/>
+      <c r="I78" s="116"/>
       <c r="J78" s="27">
         <v>1</v>
       </c>
       <c r="K78" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="L78" s="123" t="s">
+      <c r="L78" s="117" t="s">
         <v>82</v>
       </c>
-      <c r="M78" s="123"/>
-      <c r="N78" s="123"/>
+      <c r="M78" s="117"/>
+      <c r="N78" s="117"/>
       <c r="O78" s="27"/>
       <c r="P78" s="9"/>
     </row>
@@ -5235,40 +5245,40 @@
       <c r="C79" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="D79" s="121" t="s">
+      <c r="D79" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="E79" s="121"/>
-      <c r="F79" s="122"/>
-      <c r="G79" s="122"/>
-      <c r="H79" s="122"/>
-      <c r="I79" s="122"/>
+      <c r="E79" s="118"/>
+      <c r="F79" s="116"/>
+      <c r="G79" s="116"/>
+      <c r="H79" s="116"/>
+      <c r="I79" s="116"/>
       <c r="J79" s="28">
         <v>2</v>
       </c>
       <c r="K79" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="L79" s="121" t="s">
+      <c r="L79" s="118" t="s">
         <v>56</v>
       </c>
-      <c r="M79" s="121"/>
-      <c r="N79" s="121"/>
+      <c r="M79" s="118"/>
+      <c r="N79" s="118"/>
       <c r="O79" s="28"/>
       <c r="P79" s="24"/>
     </row>
     <row r="80" spans="1:17" s="22" customFormat="1" ht="25" customHeight="1">
       <c r="A80" s="47"/>
-      <c r="B80" s="183" t="s">
+      <c r="B80" s="123" t="s">
         <v>21</v>
       </c>
-      <c r="C80" s="184"/>
-      <c r="D80" s="184"/>
-      <c r="E80" s="184"/>
-      <c r="F80" s="184"/>
-      <c r="G80" s="184"/>
-      <c r="H80" s="184"/>
-      <c r="I80" s="185"/>
+      <c r="C80" s="124"/>
+      <c r="D80" s="124"/>
+      <c r="E80" s="124"/>
+      <c r="F80" s="124"/>
+      <c r="G80" s="124"/>
+      <c r="H80" s="124"/>
+      <c r="I80" s="125"/>
       <c r="J80" s="20">
         <f>SUM(J69:J71)</f>
         <v>8</v>
@@ -5334,18 +5344,18 @@
       <c r="C84" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="D84" s="182" t="s">
+      <c r="D84" s="122" t="s">
         <v>19</v>
       </c>
-      <c r="E84" s="182"/>
-      <c r="F84" s="182"/>
-      <c r="G84" s="182"/>
-      <c r="H84" s="182"/>
-      <c r="I84" s="182"/>
-      <c r="J84" s="182" t="s">
+      <c r="E84" s="122"/>
+      <c r="F84" s="122"/>
+      <c r="G84" s="122"/>
+      <c r="H84" s="122"/>
+      <c r="I84" s="122"/>
+      <c r="J84" s="122" t="s">
         <v>16</v>
       </c>
-      <c r="K84" s="182"/>
+      <c r="K84" s="122"/>
       <c r="P84" s="9"/>
     </row>
     <row r="85" spans="1:16">
@@ -5356,16 +5366,16 @@
       <c r="C85" s="29">
         <v>45486</v>
       </c>
-      <c r="D85" s="180" t="s">
+      <c r="D85" s="120" t="s">
         <v>29</v>
       </c>
-      <c r="E85" s="180"/>
-      <c r="F85" s="180"/>
-      <c r="G85" s="180"/>
-      <c r="H85" s="180"/>
-      <c r="I85" s="180"/>
-      <c r="J85" s="181"/>
-      <c r="K85" s="181"/>
+      <c r="E85" s="120"/>
+      <c r="F85" s="120"/>
+      <c r="G85" s="120"/>
+      <c r="H85" s="120"/>
+      <c r="I85" s="120"/>
+      <c r="J85" s="121"/>
+      <c r="K85" s="121"/>
       <c r="P85" s="9"/>
     </row>
     <row r="86" spans="1:16">
@@ -5376,60 +5386,60 @@
       <c r="C86" s="106">
         <v>45497</v>
       </c>
-      <c r="D86" s="186" t="s">
+      <c r="D86" s="126" t="s">
         <v>97</v>
       </c>
-      <c r="E86" s="186"/>
-      <c r="F86" s="186"/>
-      <c r="G86" s="186"/>
-      <c r="H86" s="186"/>
-      <c r="I86" s="186"/>
-      <c r="J86" s="187" t="s">
+      <c r="E86" s="126"/>
+      <c r="F86" s="126"/>
+      <c r="G86" s="126"/>
+      <c r="H86" s="126"/>
+      <c r="I86" s="126"/>
+      <c r="J86" s="127" t="s">
         <v>98</v>
       </c>
-      <c r="K86" s="187"/>
+      <c r="K86" s="127"/>
       <c r="P86" s="9"/>
     </row>
     <row r="87" spans="1:16">
       <c r="A87" s="61"/>
       <c r="B87" s="28"/>
       <c r="C87" s="29"/>
-      <c r="D87" s="180"/>
-      <c r="E87" s="180"/>
-      <c r="F87" s="180"/>
-      <c r="G87" s="180"/>
-      <c r="H87" s="180"/>
-      <c r="I87" s="180"/>
-      <c r="J87" s="181"/>
-      <c r="K87" s="181"/>
+      <c r="D87" s="120"/>
+      <c r="E87" s="120"/>
+      <c r="F87" s="120"/>
+      <c r="G87" s="120"/>
+      <c r="H87" s="120"/>
+      <c r="I87" s="120"/>
+      <c r="J87" s="121"/>
+      <c r="K87" s="121"/>
       <c r="P87" s="9"/>
     </row>
     <row r="88" spans="1:16">
       <c r="A88" s="61"/>
       <c r="B88" s="28"/>
       <c r="C88" s="29"/>
-      <c r="D88" s="180"/>
-      <c r="E88" s="180"/>
-      <c r="F88" s="180"/>
-      <c r="G88" s="180"/>
-      <c r="H88" s="180"/>
-      <c r="I88" s="180"/>
-      <c r="J88" s="181"/>
-      <c r="K88" s="181"/>
+      <c r="D88" s="120"/>
+      <c r="E88" s="120"/>
+      <c r="F88" s="120"/>
+      <c r="G88" s="120"/>
+      <c r="H88" s="120"/>
+      <c r="I88" s="120"/>
+      <c r="J88" s="121"/>
+      <c r="K88" s="121"/>
       <c r="P88" s="9"/>
     </row>
     <row r="89" spans="1:16">
       <c r="A89" s="61"/>
       <c r="B89" s="28"/>
       <c r="C89" s="30"/>
-      <c r="D89" s="180"/>
-      <c r="E89" s="180"/>
-      <c r="F89" s="180"/>
-      <c r="G89" s="180"/>
-      <c r="H89" s="180"/>
-      <c r="I89" s="180"/>
-      <c r="J89" s="181"/>
-      <c r="K89" s="181"/>
+      <c r="D89" s="120"/>
+      <c r="E89" s="120"/>
+      <c r="F89" s="120"/>
+      <c r="G89" s="120"/>
+      <c r="H89" s="120"/>
+      <c r="I89" s="120"/>
+      <c r="J89" s="121"/>
+      <c r="K89" s="121"/>
       <c r="P89" s="9"/>
     </row>
     <row r="90" spans="1:16">
@@ -6281,78 +6291,64 @@
     </row>
   </sheetData>
   <mergeCells count="154">
-    <mergeCell ref="F69:I69"/>
-    <mergeCell ref="L68:N68"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="F67:I67"/>
-    <mergeCell ref="D89:I89"/>
-    <mergeCell ref="J89:K89"/>
-    <mergeCell ref="D85:I85"/>
-    <mergeCell ref="J85:K85"/>
-    <mergeCell ref="D88:I88"/>
-    <mergeCell ref="J88:K88"/>
-    <mergeCell ref="D87:I87"/>
-    <mergeCell ref="J87:K87"/>
-    <mergeCell ref="D84:I84"/>
-    <mergeCell ref="J84:K84"/>
-    <mergeCell ref="B80:I80"/>
-    <mergeCell ref="D86:I86"/>
-    <mergeCell ref="J86:K86"/>
-    <mergeCell ref="L67:N67"/>
-    <mergeCell ref="B1:O1"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="O5:O8"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="N5:N8"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="M36:M40"/>
-    <mergeCell ref="B38:C39"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="J28:J33"/>
-    <mergeCell ref="G27:J27"/>
-    <mergeCell ref="F34:K34"/>
-    <mergeCell ref="B30:C31"/>
-    <mergeCell ref="D28:D33"/>
-    <mergeCell ref="G28:G33"/>
-    <mergeCell ref="H28:I33"/>
-    <mergeCell ref="M28:M33"/>
-    <mergeCell ref="O10:O12"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="B14:B21"/>
-    <mergeCell ref="C14:C21"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="N10:N12"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="J44:J53"/>
+    <mergeCell ref="F54:K54"/>
+    <mergeCell ref="L45:L47"/>
+    <mergeCell ref="L49:L51"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="F76:I76"/>
+    <mergeCell ref="L76:N76"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="F70:I70"/>
+    <mergeCell ref="L70:N70"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="F73:I73"/>
+    <mergeCell ref="L73:N73"/>
+    <mergeCell ref="L72:N72"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="F74:I74"/>
+    <mergeCell ref="L74:N74"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="F72:I72"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="F68:I68"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="G57:G60"/>
+    <mergeCell ref="H57:I60"/>
+    <mergeCell ref="J57:J60"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="F61:K61"/>
+    <mergeCell ref="M57:M60"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="F79:I79"/>
+    <mergeCell ref="L79:N79"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="F75:I75"/>
+    <mergeCell ref="L75:N75"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="F77:I77"/>
+    <mergeCell ref="L77:N77"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="F78:I78"/>
+    <mergeCell ref="L78:N78"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F71:I71"/>
+    <mergeCell ref="L71:N71"/>
+    <mergeCell ref="L66:N66"/>
+    <mergeCell ref="L69:N69"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="F66:I66"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="N23:N24"/>
+    <mergeCell ref="O23:O24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="L23:M23"/>
     <mergeCell ref="B46:C49"/>
     <mergeCell ref="C5:C8"/>
     <mergeCell ref="L14:M14"/>
@@ -6377,64 +6373,78 @@
     <mergeCell ref="D44:D53"/>
     <mergeCell ref="G44:G53"/>
     <mergeCell ref="H44:I53"/>
-    <mergeCell ref="N23:N24"/>
-    <mergeCell ref="O23:O24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="J57:J60"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="F61:K61"/>
-    <mergeCell ref="M57:M60"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="F79:I79"/>
-    <mergeCell ref="L79:N79"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="F75:I75"/>
-    <mergeCell ref="L75:N75"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="F77:I77"/>
-    <mergeCell ref="L77:N77"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="F78:I78"/>
-    <mergeCell ref="L78:N78"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F71:I71"/>
-    <mergeCell ref="L71:N71"/>
-    <mergeCell ref="L66:N66"/>
-    <mergeCell ref="L69:N69"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="F66:I66"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="J44:J53"/>
-    <mergeCell ref="F54:K54"/>
-    <mergeCell ref="L45:L47"/>
-    <mergeCell ref="L49:L51"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="F76:I76"/>
-    <mergeCell ref="L76:N76"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="F70:I70"/>
-    <mergeCell ref="L70:N70"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="F73:I73"/>
-    <mergeCell ref="L73:N73"/>
-    <mergeCell ref="L72:N72"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="F74:I74"/>
-    <mergeCell ref="L74:N74"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="F72:I72"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="F68:I68"/>
-    <mergeCell ref="D57:D60"/>
-    <mergeCell ref="G57:G60"/>
-    <mergeCell ref="H57:I60"/>
+    <mergeCell ref="O10:O12"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="B14:B21"/>
+    <mergeCell ref="C14:C21"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="N10:N12"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="M36:M40"/>
+    <mergeCell ref="B38:C39"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="J28:J33"/>
+    <mergeCell ref="G27:J27"/>
+    <mergeCell ref="F34:K34"/>
+    <mergeCell ref="B30:C31"/>
+    <mergeCell ref="D28:D33"/>
+    <mergeCell ref="G28:G33"/>
+    <mergeCell ref="H28:I33"/>
+    <mergeCell ref="M28:M33"/>
+    <mergeCell ref="B1:O1"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="O5:O8"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="N5:N8"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="F69:I69"/>
+    <mergeCell ref="L68:N68"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="F67:I67"/>
+    <mergeCell ref="D89:I89"/>
+    <mergeCell ref="J89:K89"/>
+    <mergeCell ref="D85:I85"/>
+    <mergeCell ref="J85:K85"/>
+    <mergeCell ref="D88:I88"/>
+    <mergeCell ref="J88:K88"/>
+    <mergeCell ref="D87:I87"/>
+    <mergeCell ref="J87:K87"/>
+    <mergeCell ref="D84:I84"/>
+    <mergeCell ref="J84:K84"/>
+    <mergeCell ref="B80:I80"/>
+    <mergeCell ref="D86:I86"/>
+    <mergeCell ref="J86:K86"/>
+    <mergeCell ref="L67:N67"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>